<commit_message>
Alterado Marcar Serviço - Especificação de Use Cases
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Marcar Serviço.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Marcar Serviço.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC328F9-0D1D-4ADF-8323-2934B410215D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF63786-E9E3-4F45-ACFD-5B234D0EC66C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{5223964D-1552-40C2-881F-30C7F509452C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Regressa a 11</t>
+  </si>
+  <si>
+    <t>Apresenta escolha do Pintor</t>
   </si>
 </sst>
 </file>
@@ -560,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DFBDAD4-08C1-4AE2-9052-6C09DB89F88C}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,20 +695,20 @@
       <c r="B13" s="1">
         <v>6</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>7</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -714,7 +717,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -724,7 +727,7 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -732,10 +735,10 @@
       <c r="B17" s="1">
         <v>10</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -743,7 +746,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -752,10 +755,10 @@
       <c r="B19" s="1">
         <v>12</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -764,7 +767,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,7 +777,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -784,85 +787,95 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B25" s="1">
         <v>1</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1">
-        <v>2</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
       <c r="B26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="B27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="B29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>